<commit_message>
Added code to impute incomplete value in every individual, refactor of some file/dir
</commit_message>
<xml_diff>
--- a/docs/Risultati per problema - FINANCIAL.xlsx
+++ b/docs/Risultati per problema - FINANCIAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATI utente\Desktop\MATERIALE TESI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATI utente\Desktop\MATERIALE TESI\MBM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323B2CBB-9352-49C4-B74D-0A555C3B2670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606C9D56-1C39-47D1-BF22-F130C0432070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{6E5E531F-E7FC-4EEA-950F-50312C97E849}"/>
+    <workbookView xWindow="26175" yWindow="4125" windowWidth="21600" windowHeight="11430" xr2:uid="{6E5E531F-E7FC-4EEA-950F-50312C97E849}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
   <si>
     <t>KNOWLEDGE GRAPH: FINANCIAL</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>0.944 ± 0.070</t>
+  </si>
+  <si>
+    <t>0.971 ± 0.048</t>
+  </si>
+  <si>
+    <t>0.958 ± 0.065</t>
+  </si>
+  <si>
+    <t>0.987 ± 0.066</t>
+  </si>
+  <si>
+    <t>CON DATI IMPUTATI</t>
   </si>
 </sst>
 </file>
@@ -398,12 +410,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,6 +485,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,66 +498,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -794,7 +806,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -802,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBEF0CE-B705-41D3-94E7-D231E1DE1EB2}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,832 +826,932 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="15">
+      <c r="D3" s="23"/>
+      <c r="E3" s="24">
         <v>56</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="16"/>
+      <c r="H3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="21"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33">
+      <c r="D4" s="6"/>
+      <c r="E4" s="7">
         <v>505</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="17"/>
+      <c r="H4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="22" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="5">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11">
         <v>439</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="6"/>
+      <c r="H5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="15">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24">
         <v>137</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="H6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="16"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33">
+      <c r="D7" s="6"/>
+      <c r="E7" s="7">
         <v>623</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33" t="s">
+      <c r="H7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="17"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33">
+      <c r="D8" s="6"/>
+      <c r="E8" s="7">
         <v>240</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="s">
+      <c r="H8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="17"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="15">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24">
         <v>381</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15" t="s">
+      <c r="H9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="16"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="21"/>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33">
+      <c r="D10" s="6"/>
+      <c r="E10" s="7">
         <v>379</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33" t="s">
+      <c r="H10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="5">
+      <c r="D11" s="10"/>
+      <c r="E11" s="11">
         <v>240</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="15">
+      <c r="D12" s="23"/>
+      <c r="E12" s="24">
         <v>255</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="16"/>
+      <c r="H12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33">
+      <c r="D13" s="6"/>
+      <c r="E13" s="7">
         <v>505</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="17"/>
+      <c r="H13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="22" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="5">
+      <c r="D14" s="10"/>
+      <c r="E14" s="11">
         <v>240</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="6"/>
+      <c r="H14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="15">
+      <c r="D15" s="23"/>
+      <c r="E15" s="24">
         <v>255</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" s="16"/>
+      <c r="H15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33">
+      <c r="D16" s="6"/>
+      <c r="E16" s="7">
         <v>505</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="17"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="22" t="s">
+      <c r="H16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="5">
+      <c r="D17" s="10"/>
+      <c r="E17" s="11">
         <v>240</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="H17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="15">
+      <c r="D18" s="23"/>
+      <c r="E18" s="24">
         <v>217</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="H18" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
       <c r="B19" s="21"/>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="33">
+      <c r="D19" s="6"/>
+      <c r="E19" s="7">
         <v>505</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="22" t="s">
+      <c r="H19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="5">
+      <c r="D20" s="10"/>
+      <c r="E20" s="11">
         <v>278</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="H20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="15">
+      <c r="D21" s="23"/>
+      <c r="E21" s="24">
         <v>8</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33">
+      <c r="D22" s="6"/>
+      <c r="E22" s="7">
         <v>752</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33" t="s">
+      <c r="I22" s="7"/>
+      <c r="J22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="22" t="s">
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="5">
+      <c r="D23" s="10"/>
+      <c r="E23" s="11">
         <v>240</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5" t="s">
+      <c r="I23" s="11"/>
+      <c r="J23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="15">
+      <c r="D24" s="23"/>
+      <c r="E24" s="24">
         <v>255</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="H24" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="25"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
       <c r="B25" s="21"/>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33">
+      <c r="D25" s="6"/>
+      <c r="E25" s="7">
         <v>505</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="22" t="s">
+      <c r="H25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="5">
+      <c r="D26" s="10"/>
+      <c r="E26" s="11">
         <v>240</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+      <c r="H26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="15">
+      <c r="D27" s="23"/>
+      <c r="E27" s="24">
         <v>381</v>
       </c>
-      <c r="F27" s="16"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15" t="s">
+      <c r="H27" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
+      <c r="K27" s="25"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
       <c r="B28" s="21"/>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33">
+      <c r="D28" s="6"/>
+      <c r="E28" s="7">
         <v>379</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33" t="s">
+      <c r="H28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K28" s="17"/>
-    </row>
-    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="22" t="s">
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="5">
+      <c r="D29" s="10"/>
+      <c r="E29" s="11">
         <v>240</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5" t="s">
+      <c r="H29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="15">
+      <c r="D30" s="23"/>
+      <c r="E30" s="24">
         <v>56</v>
       </c>
-      <c r="F30" s="16"/>
+      <c r="F30" s="25"/>
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="I30" s="24"/>
+      <c r="J30" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="16"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
+      <c r="K30" s="25"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
       <c r="B31" s="21"/>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="33">
+      <c r="D31" s="6"/>
+      <c r="E31" s="7">
         <v>704</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="H31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33" t="s">
+      <c r="I31" s="7"/>
+      <c r="J31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K31" s="17"/>
-    </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="22" t="s">
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="5">
+      <c r="D32" s="10"/>
+      <c r="E32" s="11">
         <v>240</v>
       </c>
-      <c r="F32" s="6"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5" t="s">
+      <c r="I32" s="11"/>
+      <c r="J32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="K32" s="12"/>
+      <c r="L32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15" t="s">
+      <c r="I33" s="24"/>
+      <c r="J33" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="11"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M33" s="25"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="33" t="s">
+      <c r="H34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33" t="s">
+      <c r="I34" s="7"/>
+      <c r="J34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="14"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5" t="s">
+      <c r="I35" s="11"/>
+      <c r="J35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="142">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
+  <mergeCells count="145">
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="A33:F35"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="A27:B29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A21:B23"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A18:B20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="A9:B11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
@@ -1664,106 +1776,24 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A21:B23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="A27:B29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A24:B26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A33:F35"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>